<commit_message>
Création stratégies d'alignement et validation en cours voir fichier Excel.
</commit_message>
<xml_diff>
--- a/_01-docs/_01-userDoc/documentionProjetToWeb/source/advanced/simplificationCapteur191214_1518.xlsx
+++ b/_01-docs/_01-userDoc/documentionProjetToWeb/source/advanced/simplificationCapteur191214_1518.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MountWD\Donnees\ODJ\008_iao_wrk\VoRoboticsAsso\00-AutresProjetsDuLab\0025-permiC_2019\project\_01-docs\_01-userDoc\documentionProjetToWeb\source\advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459368FE-300E-426B-BF06-F685E31553AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C220D13C-8E73-40B3-987E-1DCA500A0F88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="1" xr2:uid="{85A47218-88F4-4F6A-A7B0-57E7AE9DD31F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="23">
   <si>
     <t>NON</t>
   </si>
@@ -83,6 +83,24 @@
   </si>
   <si>
     <t>S1 est valide à la fois pour côté droit et gauche</t>
+  </si>
+  <si>
+    <t>angle d'incidence compris entre 75° et 30°</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>Avance 80mm puis tourne</t>
+  </si>
+  <si>
+    <t>S0</t>
+  </si>
+  <si>
+    <t>Incidence max 65°</t>
+  </si>
+  <si>
+    <t>S0 même avec incidence max : 50°</t>
   </si>
 </sst>
 </file>
@@ -2339,10 +2357,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E56ABBBC-22BD-47C7-9A9F-76F52387221E}">
-  <dimension ref="A1:R50"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2363,13 +2381,13 @@
     <col min="16" max="16" width="4.42578125" customWidth="1"/>
     <col min="17" max="17" width="6.7109375" customWidth="1"/>
     <col min="18" max="18" width="16.28515625" customWidth="1"/>
-    <col min="19" max="19" width="4.7109375" customWidth="1"/>
+    <col min="19" max="19" width="42.5703125" customWidth="1"/>
     <col min="20" max="20" width="4.28515625" customWidth="1"/>
     <col min="21" max="21" width="7" customWidth="1"/>
     <col min="22" max="22" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2388,7 +2406,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2426,7 +2444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2481,7 +2499,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2532,8 +2550,11 @@
       <c r="Q4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2584,8 +2605,14 @@
       <c r="Q5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>18</v>
+      </c>
+      <c r="S5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2639,8 +2666,14 @@
       <c r="Q6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>20</v>
+      </c>
+      <c r="S6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -2691,8 +2724,14 @@
       <c r="Q7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R7" t="s">
+        <v>18</v>
+      </c>
+      <c r="S7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2744,7 +2783,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12</v>
       </c>
@@ -2796,7 +2835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>14</v>
       </c>
@@ -2848,7 +2887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15</v>
       </c>
@@ -2900,7 +2939,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>17</v>
       </c>
@@ -2952,7 +2991,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>25</v>
       </c>
@@ -3004,7 +3043,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>26</v>
       </c>
@@ -3056,7 +3095,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>36</v>
       </c>
@@ -3122,6 +3161,14 @@
       </c>
       <c r="K18" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tous les cas testé et validés avec 3 stratégies S0, S1, S2 souf 0,0
</commit_message>
<xml_diff>
--- a/_01-docs/_01-userDoc/documentionProjetToWeb/source/advanced/simplificationCapteur191214_1518.xlsx
+++ b/_01-docs/_01-userDoc/documentionProjetToWeb/source/advanced/simplificationCapteur191214_1518.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MountWD\Donnees\ODJ\008_iao_wrk\VoRoboticsAsso\00-AutresProjetsDuLab\0025-permiC_2019\project\_01-docs\_01-userDoc\documentionProjetToWeb\source\advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C220D13C-8E73-40B3-987E-1DCA500A0F88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C2062C-6EEF-43AD-BA61-6D6D888D7B05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="1" xr2:uid="{85A47218-88F4-4F6A-A7B0-57E7AE9DD31F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="34">
   <si>
     <t>NON</t>
   </si>
@@ -102,6 +102,39 @@
   <si>
     <t>S0 même avec incidence max : 50°</t>
   </si>
+  <si>
+    <t>Gch</t>
+  </si>
+  <si>
+    <t>Drt</t>
+  </si>
+  <si>
+    <t>incidence max 75°</t>
+  </si>
+  <si>
+    <t>Pas vriament de besoin d'alignement</t>
+  </si>
+  <si>
+    <t>Attention les capteurs retournent 1,2,4 en partant du centre</t>
+  </si>
+  <si>
+    <t>incidence max 77°</t>
+  </si>
+  <si>
+    <t>S2 mais en déplaçant le ou 1,1 à la fin après les autres test</t>
+  </si>
+  <si>
+    <t>incidence max 85°</t>
+  </si>
+  <si>
+    <t>éliminé : fourche</t>
+  </si>
+  <si>
+    <t>incidence max 74°</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
 </sst>
 </file>
 
@@ -163,10 +196,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,10 +533,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="6"/>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" t="s">
@@ -2357,10 +2390,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E56ABBBC-22BD-47C7-9A9F-76F52387221E}">
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2387,18 +2420,22 @@
     <col min="22" max="22" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="L1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
+      <c r="G1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
       <c r="Q1" t="s">
         <v>11</v>
       </c>
@@ -2406,7 +2443,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2417,26 +2454,26 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="str">
-        <f>DEC2BIN(B2, 3)</f>
+        <f t="shared" ref="D2:D15" si="0">DEC2BIN(B2, 3)</f>
         <v>000</v>
       </c>
       <c r="E2" s="1" t="str">
-        <f>DEC2BIN(C2, 3)</f>
+        <f t="shared" ref="E2:E15" si="1">DEC2BIN(C2, 3)</f>
         <v>000</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="6">
         <f>IF(C2=0,0,IF(C2=1,4,IF(C2=2,2,IF(C2=3,6,IF(C2=4,1,IF(C2=5,5,IF(C2=6,3,IF(C2=7,7,255))))))))</f>
         <v>0</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="6">
         <f>IF(B2=0,0,IF(B2=1,4,IF(B2=2,2,IF(B2=3,6,IF(B2=4,1,IF(B2=5,5,IF(B2=6,3,IF(B2=7,7,255))))))))</f>
         <v>0</v>
       </c>
-      <c r="N2" s="7" t="str">
+      <c r="N2" s="6" t="str">
         <f>IF(AND(B2=L2,C2=M2),"EGAL","")</f>
         <v>EGAL</v>
       </c>
-      <c r="O2" s="7" t="str">
+      <c r="O2" s="6" t="str">
         <f>IF(AND(G2=L2,H2=M2),"BON","")</f>
         <v>BON</v>
       </c>
@@ -2444,7 +2481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2455,11 +2492,11 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f>DEC2BIN(B3, 3)</f>
+        <f t="shared" si="0"/>
         <v>000</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f>DEC2BIN(C3, 3)</f>
+        <f t="shared" si="1"/>
         <v>001</v>
       </c>
       <c r="G3">
@@ -2469,27 +2506,27 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f>DEC2BIN(G3, 3)</f>
+        <f t="shared" ref="I3:I15" si="2">DEC2BIN(G3, 3)</f>
         <v>100</v>
       </c>
       <c r="J3" s="1" t="str">
-        <f>DEC2BIN(H3, 3)</f>
+        <f t="shared" ref="J3:J15" si="3">DEC2BIN(H3, 3)</f>
         <v>000</v>
       </c>
-      <c r="L3" s="7">
-        <f t="shared" ref="L3:L16" si="0">IF(C3=0,0,IF(C3=1,4,IF(C3=2,2,IF(C3=3,6,IF(C3=4,1,IF(C3=5,5,IF(C3=6,3,IF(C3=7,7,255))))))))</f>
-        <v>4</v>
-      </c>
-      <c r="M3" s="7">
-        <f t="shared" ref="M3:M16" si="1">IF(B3=0,0,IF(B3=1,4,IF(B3=2,2,IF(B3=3,6,IF(B3=4,1,IF(B3=5,5,IF(B3=6,3,IF(B3=7,7,255))))))))</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="7" t="str">
-        <f t="shared" ref="N3:N16" si="2">IF(AND(B3=L3,C3=M3),"EGAL","")</f>
+      <c r="L3" s="6">
+        <f t="shared" ref="L3:L14" si="4">IF(C3=0,0,IF(C3=1,4,IF(C3=2,2,IF(C3=3,6,IF(C3=4,1,IF(C3=5,5,IF(C3=6,3,IF(C3=7,7,255))))))))</f>
+        <v>4</v>
+      </c>
+      <c r="M3" s="6">
+        <f t="shared" ref="M3:M14" si="5">IF(B3=0,0,IF(B3=1,4,IF(B3=2,2,IF(B3=3,6,IF(B3=4,1,IF(B3=5,5,IF(B3=6,3,IF(B3=7,7,255))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="6" t="str">
+        <f t="shared" ref="N3:N14" si="6">IF(AND(B3=L3,C3=M3),"EGAL","")</f>
         <v/>
       </c>
-      <c r="O3" s="7" t="str">
-        <f t="shared" ref="O3:O16" si="3">IF(AND(G3=L3,H3=M3),"BON","")</f>
+      <c r="O3" s="6" t="str">
+        <f t="shared" ref="O3:O14" si="7">IF(AND(G3=L3,H3=M3),"BON","")</f>
         <v>BON</v>
       </c>
       <c r="Q3">
@@ -2499,7 +2536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2510,11 +2547,11 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="str">
-        <f>DEC2BIN(B4, 3)</f>
+        <f t="shared" si="0"/>
         <v>000</v>
       </c>
       <c r="E4" s="1" t="str">
-        <f>DEC2BIN(C4, 3)</f>
+        <f t="shared" si="1"/>
         <v>010</v>
       </c>
       <c r="G4">
@@ -2524,27 +2561,27 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>DEC2BIN(G4, 3)</f>
+        <f t="shared" si="2"/>
         <v>010</v>
       </c>
       <c r="J4" s="1" t="str">
-        <f>DEC2BIN(H4, 3)</f>
+        <f t="shared" si="3"/>
         <v>000</v>
       </c>
-      <c r="L4" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="M4" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N4" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="L4" s="6">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="M4" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N4" s="6" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="O4" s="7" t="str">
-        <f t="shared" si="3"/>
+      <c r="O4" s="6" t="str">
+        <f t="shared" si="7"/>
         <v>BON</v>
       </c>
       <c r="Q4">
@@ -2554,7 +2591,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2565,11 +2602,11 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="str">
-        <f>DEC2BIN(B5, 3)</f>
+        <f t="shared" si="0"/>
         <v>000</v>
       </c>
       <c r="E5" s="1" t="str">
-        <f>DEC2BIN(C5, 3)</f>
+        <f t="shared" si="1"/>
         <v>011</v>
       </c>
       <c r="G5">
@@ -2579,27 +2616,27 @@
         <v>0</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f>DEC2BIN(G5, 3)</f>
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
       <c r="J5" s="1" t="str">
-        <f>DEC2BIN(H5, 3)</f>
+        <f t="shared" si="3"/>
         <v>000</v>
       </c>
-      <c r="L5" s="7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="M5" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N5" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="L5" s="6">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="M5" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="6" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="O5" s="7" t="str">
-        <f t="shared" si="3"/>
+      <c r="O5" s="6" t="str">
+        <f t="shared" si="7"/>
         <v>BON</v>
       </c>
       <c r="Q5">
@@ -2612,7 +2649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2623,11 +2660,11 @@
         <v>4</v>
       </c>
       <c r="D6" s="1" t="str">
-        <f>DEC2BIN(B6, 3)</f>
+        <f t="shared" si="0"/>
         <v>000</v>
       </c>
       <c r="E6" s="1" t="str">
-        <f>DEC2BIN(C6, 3)</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G6">
@@ -2637,27 +2674,27 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f>DEC2BIN(G6, 3)</f>
+        <f t="shared" si="2"/>
         <v>001</v>
       </c>
       <c r="J6" s="1" t="str">
-        <f>DEC2BIN(H6, 3)</f>
+        <f t="shared" si="3"/>
         <v>000</v>
       </c>
-      <c r="L6" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M6" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N6" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="L6" s="6">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M6" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="6" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="O6" s="7" t="str">
-        <f t="shared" si="3"/>
+      <c r="O6" s="6" t="str">
+        <f t="shared" si="7"/>
         <v>BON</v>
       </c>
       <c r="P6" t="s">
@@ -2673,7 +2710,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -2684,11 +2721,11 @@
         <v>6</v>
       </c>
       <c r="D7" s="1" t="str">
-        <f>DEC2BIN(B7, 3)</f>
+        <f t="shared" si="0"/>
         <v>000</v>
       </c>
       <c r="E7" s="1" t="str">
-        <f>DEC2BIN(C7, 3)</f>
+        <f t="shared" si="1"/>
         <v>110</v>
       </c>
       <c r="G7">
@@ -2698,27 +2735,27 @@
         <v>0</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f>DEC2BIN(G7, 3)</f>
+        <f t="shared" si="2"/>
         <v>011</v>
       </c>
       <c r="J7" s="1" t="str">
-        <f>DEC2BIN(H7, 3)</f>
+        <f t="shared" si="3"/>
         <v>000</v>
       </c>
-      <c r="L7" s="7">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="M7" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N7" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="L7" s="6">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="M7" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="6" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="O7" s="7" t="str">
-        <f t="shared" si="3"/>
+      <c r="O7" s="6" t="str">
+        <f t="shared" si="7"/>
         <v>BON</v>
       </c>
       <c r="Q7">
@@ -2731,7 +2768,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2742,11 +2779,11 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="str">
-        <f>DEC2BIN(B8, 3)</f>
+        <f t="shared" si="0"/>
         <v>000</v>
       </c>
       <c r="E8" s="1" t="str">
-        <f>DEC2BIN(C8, 3)</f>
+        <f t="shared" si="1"/>
         <v>111</v>
       </c>
       <c r="G8">
@@ -2756,34 +2793,40 @@
         <v>0</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f>DEC2BIN(G8, 3)</f>
+        <f t="shared" si="2"/>
         <v>111</v>
       </c>
       <c r="J8" s="1" t="str">
-        <f>DEC2BIN(H8, 3)</f>
+        <f t="shared" si="3"/>
         <v>000</v>
       </c>
-      <c r="L8" s="7">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="M8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="7" t="str">
-        <f t="shared" si="2"/>
+      <c r="L8" s="6">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="M8" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="6" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="O8" s="7" t="str">
-        <f t="shared" si="3"/>
+      <c r="O8" s="6" t="str">
+        <f t="shared" si="7"/>
         <v>BON</v>
       </c>
       <c r="Q8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R8" t="s">
+        <v>18</v>
+      </c>
+      <c r="S8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12</v>
       </c>
@@ -2794,11 +2837,11 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="str">
-        <f>DEC2BIN(B9, 3)</f>
+        <f t="shared" si="0"/>
         <v>001</v>
       </c>
       <c r="E9" s="1" t="str">
-        <f>DEC2BIN(C9, 3)</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="G9">
@@ -2808,34 +2851,40 @@
         <v>4</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>DEC2BIN(G9, 3)</f>
+        <f t="shared" si="2"/>
         <v>001</v>
       </c>
       <c r="J9" s="1" t="str">
-        <f>DEC2BIN(H9, 3)</f>
-        <v>100</v>
-      </c>
-      <c r="L9" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M9" s="7">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="N9" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="L9" s="6">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M9" s="6">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="N9" s="6" t="str">
+        <f t="shared" si="6"/>
         <v>EGAL</v>
       </c>
-      <c r="O9" s="7" t="str">
-        <f t="shared" si="3"/>
+      <c r="O9" s="6" t="str">
+        <f t="shared" si="7"/>
         <v>BON</v>
       </c>
       <c r="Q9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R9" t="s">
+        <v>20</v>
+      </c>
+      <c r="S9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>14</v>
       </c>
@@ -2846,11 +2895,11 @@
         <v>6</v>
       </c>
       <c r="D10" s="1" t="str">
-        <f>DEC2BIN(B10, 3)</f>
+        <f t="shared" si="0"/>
         <v>001</v>
       </c>
       <c r="E10" s="1" t="str">
-        <f>DEC2BIN(C10, 3)</f>
+        <f t="shared" si="1"/>
         <v>110</v>
       </c>
       <c r="G10">
@@ -2860,34 +2909,43 @@
         <v>4</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f>DEC2BIN(G10, 3)</f>
+        <f t="shared" si="2"/>
         <v>011</v>
       </c>
       <c r="J10" s="1" t="str">
-        <f>DEC2BIN(H10, 3)</f>
-        <v>100</v>
-      </c>
-      <c r="L10" s="7">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="M10" s="7">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="N10" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="L10" s="6">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="M10" s="6">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="N10" s="6" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="O10" s="7" t="str">
-        <f t="shared" si="3"/>
+      <c r="O10" s="6" t="str">
+        <f t="shared" si="7"/>
         <v>BON</v>
       </c>
       <c r="Q10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R10" t="s">
+        <v>18</v>
+      </c>
+      <c r="S10" t="s">
+        <v>28</v>
+      </c>
+      <c r="T10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15</v>
       </c>
@@ -2898,11 +2956,11 @@
         <v>7</v>
       </c>
       <c r="D11" s="1" t="str">
-        <f>DEC2BIN(B11, 3)</f>
+        <f t="shared" si="0"/>
         <v>001</v>
       </c>
       <c r="E11" s="1" t="str">
-        <f>DEC2BIN(C11, 3)</f>
+        <f t="shared" si="1"/>
         <v>111</v>
       </c>
       <c r="G11">
@@ -2912,34 +2970,40 @@
         <v>4</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f>DEC2BIN(G11, 3)</f>
+        <f t="shared" si="2"/>
         <v>111</v>
       </c>
       <c r="J11" s="1" t="str">
-        <f>DEC2BIN(H11, 3)</f>
-        <v>100</v>
-      </c>
-      <c r="L11" s="7">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="M11" s="7">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="N11" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="L11" s="6">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="M11" s="6">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="N11" s="6" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="O11" s="7" t="str">
-        <f t="shared" si="3"/>
+      <c r="O11" s="6" t="str">
+        <f t="shared" si="7"/>
         <v>BON</v>
       </c>
       <c r="Q11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R11" t="s">
+        <v>18</v>
+      </c>
+      <c r="S11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>17</v>
       </c>
@@ -2950,11 +3014,11 @@
         <v>2</v>
       </c>
       <c r="D12" s="1" t="str">
-        <f>DEC2BIN(B12, 3)</f>
+        <f t="shared" si="0"/>
         <v>010</v>
       </c>
       <c r="E12" s="1" t="str">
-        <f>DEC2BIN(C12, 3)</f>
+        <f t="shared" si="1"/>
         <v>010</v>
       </c>
       <c r="G12">
@@ -2964,34 +3028,37 @@
         <v>2</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f>DEC2BIN(G12, 3)</f>
+        <f t="shared" si="2"/>
         <v>010</v>
       </c>
       <c r="J12" s="1" t="str">
-        <f>DEC2BIN(H12, 3)</f>
-        <v>010</v>
-      </c>
-      <c r="L12" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="M12" s="7">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="N12" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>010</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="M12" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="N12" s="6" t="str">
+        <f t="shared" si="6"/>
         <v>EGAL</v>
       </c>
-      <c r="O12" s="7" t="str">
-        <f t="shared" si="3"/>
+      <c r="O12" s="6" t="str">
+        <f t="shared" si="7"/>
         <v>BON</v>
       </c>
       <c r="Q12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>25</v>
       </c>
@@ -3002,11 +3069,11 @@
         <v>6</v>
       </c>
       <c r="D13" s="1" t="str">
-        <f>DEC2BIN(B13, 3)</f>
+        <f t="shared" si="0"/>
         <v>011</v>
       </c>
       <c r="E13" s="1" t="str">
-        <f>DEC2BIN(C13, 3)</f>
+        <f t="shared" si="1"/>
         <v>110</v>
       </c>
       <c r="G13">
@@ -3016,34 +3083,40 @@
         <v>6</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f>DEC2BIN(G13, 3)</f>
+        <f t="shared" si="2"/>
         <v>011</v>
       </c>
       <c r="J13" s="1" t="str">
-        <f>DEC2BIN(H13, 3)</f>
-        <v>110</v>
-      </c>
-      <c r="L13" s="7">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="M13" s="7">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="N13" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>110</v>
+      </c>
+      <c r="L13" s="6">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="M13" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="N13" s="6" t="str">
+        <f t="shared" si="6"/>
         <v>EGAL</v>
       </c>
-      <c r="O13" s="7" t="str">
-        <f t="shared" si="3"/>
+      <c r="O13" s="6" t="str">
+        <f t="shared" si="7"/>
         <v>BON</v>
       </c>
       <c r="Q13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R13" t="s">
+        <v>18</v>
+      </c>
+      <c r="S13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>26</v>
       </c>
@@ -3054,11 +3127,11 @@
         <v>7</v>
       </c>
       <c r="D14" s="1" t="str">
-        <f>DEC2BIN(B14, 3)</f>
+        <f t="shared" si="0"/>
         <v>011</v>
       </c>
       <c r="E14" s="1" t="str">
-        <f>DEC2BIN(C14, 3)</f>
+        <f t="shared" si="1"/>
         <v>111</v>
       </c>
       <c r="G14">
@@ -3068,34 +3141,37 @@
         <v>6</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f>DEC2BIN(G14, 3)</f>
+        <f t="shared" si="2"/>
         <v>111</v>
       </c>
       <c r="J14" s="1" t="str">
-        <f>DEC2BIN(H14, 3)</f>
-        <v>110</v>
-      </c>
-      <c r="L14" s="7">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="M14" s="7">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="N14" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>110</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="M14" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="N14" s="6" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="O14" s="7" t="str">
-        <f t="shared" si="3"/>
+      <c r="O14" s="6" t="str">
+        <f t="shared" si="7"/>
         <v>BON</v>
       </c>
       <c r="Q14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>36</v>
       </c>
@@ -3106,11 +3182,11 @@
         <v>7</v>
       </c>
       <c r="D15" s="1" t="str">
-        <f>DEC2BIN(B15, 3)</f>
+        <f t="shared" si="0"/>
         <v>111</v>
       </c>
       <c r="E15" s="1" t="str">
-        <f>DEC2BIN(C15, 3)</f>
+        <f t="shared" si="1"/>
         <v>111</v>
       </c>
       <c r="G15">
@@ -3120,1253 +3196,1265 @@
         <v>7</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>DEC2BIN(G15, 3)</f>
+        <f t="shared" si="2"/>
         <v>111</v>
       </c>
       <c r="J15" s="1" t="str">
-        <f>DEC2BIN(H15, 3)</f>
+        <f t="shared" si="3"/>
         <v>111</v>
       </c>
-      <c r="L15" s="7">
-        <f t="shared" ref="L15" si="4">IF(C15=0,0,IF(C15=1,4,IF(C15=2,2,IF(C15=3,6,IF(C15=4,1,IF(C15=5,5,IF(C15=6,3,IF(C15=7,7,255))))))))</f>
-        <v>7</v>
-      </c>
-      <c r="M15" s="7">
-        <f t="shared" ref="M15" si="5">IF(B15=0,0,IF(B15=1,4,IF(B15=2,2,IF(B15=3,6,IF(B15=4,1,IF(B15=5,5,IF(B15=6,3,IF(B15=7,7,255))))))))</f>
-        <v>7</v>
-      </c>
-      <c r="N15" s="7" t="str">
-        <f t="shared" ref="N15" si="6">IF(AND(B15=L15,C15=M15),"EGAL","")</f>
+      <c r="L15" s="6">
+        <f t="shared" ref="L15" si="8">IF(C15=0,0,IF(C15=1,4,IF(C15=2,2,IF(C15=3,6,IF(C15=4,1,IF(C15=5,5,IF(C15=6,3,IF(C15=7,7,255))))))))</f>
+        <v>7</v>
+      </c>
+      <c r="M15" s="6">
+        <f t="shared" ref="M15" si="9">IF(B15=0,0,IF(B15=1,4,IF(B15=2,2,IF(B15=3,6,IF(B15=4,1,IF(B15=5,5,IF(B15=6,3,IF(B15=7,7,255))))))))</f>
+        <v>7</v>
+      </c>
+      <c r="N15" s="6" t="str">
+        <f t="shared" ref="N15" si="10">IF(AND(B15=L15,C15=M15),"EGAL","")</f>
         <v>EGAL</v>
       </c>
-      <c r="O15" s="7" t="str">
-        <f t="shared" ref="O15" si="7">IF(AND(G15=L15,H15=M15),"BON","")</f>
+      <c r="O15" s="6" t="str">
+        <f t="shared" ref="O15" si="11">IF(AND(G15=L15,H15=M15),"BON","")</f>
         <v>BON</v>
       </c>
       <c r="Q15">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
+      <c r="R15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="K18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>6</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>5</v>
-      </c>
-      <c r="D24" s="1" t="str">
-        <f>DEC2BIN(B24, 3)</f>
-        <v>000</v>
-      </c>
-      <c r="E24" s="1" t="str">
-        <f>DEC2BIN(C24, 3)</f>
-        <v>101</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>5</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1" t="str">
-        <f>DEC2BIN(G24, 3)</f>
-        <v>101</v>
-      </c>
-      <c r="J24" s="1" t="str">
-        <f>DEC2BIN(H24, 3)</f>
-        <v>000</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L24" s="7">
-        <f>IF(C24=0,0,IF(C24=1,4,IF(C24=2,2,IF(C24=3,6,IF(C24=4,1,IF(C24=5,5,IF(C24=6,3,IF(C24=7,7,255))))))))</f>
-        <v>5</v>
-      </c>
-      <c r="M24" s="7">
-        <f>IF(B24=0,0,IF(B24=1,4,IF(B24=2,2,IF(B24=3,6,IF(B24=4,1,IF(B24=5,5,IF(B24=6,3,IF(B24=7,7,255))))))))</f>
-        <v>0</v>
-      </c>
-      <c r="N24" s="7" t="str">
-        <f>IF(AND(B24=L24,C24=M24),"EGAL","")</f>
-        <v/>
-      </c>
-      <c r="O24" s="7" t="str">
-        <f>IF(AND(G24=L24,H24=M24),"BON","")</f>
-        <v>BON</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D25" s="1" t="str">
-        <f>DEC2BIN(B25, 3)</f>
-        <v>001</v>
+        <f t="shared" ref="D25:D46" si="12">DEC2BIN(B25, 3)</f>
+        <v>000</v>
       </c>
       <c r="E25" s="1" t="str">
-        <f>DEC2BIN(C25, 3)</f>
-        <v>001</v>
+        <f t="shared" ref="E25:E46" si="13">DEC2BIN(C25, 3)</f>
+        <v>101</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f>DEC2BIN(G25, 3)</f>
-        <v>100</v>
+        <f t="shared" ref="I25:I46" si="14">DEC2BIN(G25, 3)</f>
+        <v>101</v>
       </c>
       <c r="J25" s="1" t="str">
-        <f>DEC2BIN(H25, 3)</f>
-        <v>100</v>
-      </c>
-      <c r="K25" t="s">
-        <v>6</v>
-      </c>
-      <c r="L25" s="7">
-        <f>IF(C25=0,0,IF(C25=1,4,IF(C25=2,2,IF(C25=3,6,IF(C25=4,1,IF(C25=5,5,IF(C25=6,3,IF(C25=7,7,255))))))))</f>
-        <v>4</v>
-      </c>
-      <c r="M25" s="7">
-        <f>IF(B25=0,0,IF(B25=1,4,IF(B25=2,2,IF(B25=3,6,IF(B25=4,1,IF(B25=5,5,IF(B25=6,3,IF(B25=7,7,255))))))))</f>
-        <v>4</v>
-      </c>
-      <c r="N25" s="7" t="str">
-        <f>IF(AND(B25=L25,C25=M25),"EGAL","")</f>
+        <f t="shared" ref="J25:J46" si="15">DEC2BIN(H25, 3)</f>
+        <v>000</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25" s="6">
+        <f t="shared" ref="L25:L42" si="16">IF(C25=0,0,IF(C25=1,4,IF(C25=2,2,IF(C25=3,6,IF(C25=4,1,IF(C25=5,5,IF(C25=6,3,IF(C25=7,7,255))))))))</f>
+        <v>5</v>
+      </c>
+      <c r="M25" s="6">
+        <f t="shared" ref="M25:M42" si="17">IF(B25=0,0,IF(B25=1,4,IF(B25=2,2,IF(B25=3,6,IF(B25=4,1,IF(B25=5,5,IF(B25=6,3,IF(B25=7,7,255))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="6" t="str">
+        <f t="shared" ref="N25:N42" si="18">IF(AND(B25=L25,C25=M25),"EGAL","")</f>
         <v/>
       </c>
-      <c r="O25" s="7" t="str">
-        <f>IF(AND(G25=L25,H25=M25),"BON","")</f>
+      <c r="O25" s="6" t="str">
+        <f t="shared" ref="O25:O43" si="19">IF(AND(G25=L25,H25=M25),"BON","")</f>
         <v>BON</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1" t="str">
-        <f>DEC2BIN(B26, 3)</f>
+        <f t="shared" si="12"/>
         <v>001</v>
       </c>
       <c r="E26" s="1" t="str">
-        <f>DEC2BIN(C26, 3)</f>
-        <v>010</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>001</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H26">
         <v>4</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f>DEC2BIN(G26, 3)</f>
-        <v>010</v>
+        <f t="shared" si="14"/>
+        <v>100</v>
       </c>
       <c r="J26" s="1" t="str">
-        <f>DEC2BIN(H26, 3)</f>
-        <v>100</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L26" s="7">
-        <f>IF(C26=0,0,IF(C26=1,4,IF(C26=2,2,IF(C26=3,6,IF(C26=4,1,IF(C26=5,5,IF(C26=6,3,IF(C26=7,7,255))))))))</f>
-        <v>2</v>
-      </c>
-      <c r="M26" s="7">
-        <f>IF(B26=0,0,IF(B26=1,4,IF(B26=2,2,IF(B26=3,6,IF(B26=4,1,IF(B26=5,5,IF(B26=6,3,IF(B26=7,7,255))))))))</f>
-        <v>4</v>
-      </c>
-      <c r="N26" s="7" t="str">
-        <f>IF(AND(B26=L26,C26=M26),"EGAL","")</f>
+        <f t="shared" si="15"/>
+        <v>100</v>
+      </c>
+      <c r="K26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L26" s="6">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="M26" s="6">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="N26" s="6" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="O26" s="7" t="str">
-        <f>IF(AND(G26=L26,H26=M26),"BON","")</f>
+      <c r="O26" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27" s="1" t="str">
-        <f>DEC2BIN(B27, 3)</f>
+        <f t="shared" si="12"/>
         <v>001</v>
       </c>
       <c r="E27" s="1" t="str">
-        <f>DEC2BIN(C27, 3)</f>
-        <v>011</v>
+        <f t="shared" si="13"/>
+        <v>010</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G27">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H27">
         <v>4</v>
       </c>
       <c r="I27" s="1" t="str">
-        <f>DEC2BIN(G27, 3)</f>
-        <v>110</v>
+        <f t="shared" si="14"/>
+        <v>010</v>
       </c>
       <c r="J27" s="1" t="str">
-        <f>DEC2BIN(H27, 3)</f>
+        <f t="shared" si="15"/>
         <v>100</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L27" s="7">
-        <f>IF(C27=0,0,IF(C27=1,4,IF(C27=2,2,IF(C27=3,6,IF(C27=4,1,IF(C27=5,5,IF(C27=6,3,IF(C27=7,7,255))))))))</f>
-        <v>6</v>
-      </c>
-      <c r="M27" s="7">
-        <f>IF(B27=0,0,IF(B27=1,4,IF(B27=2,2,IF(B27=3,6,IF(B27=4,1,IF(B27=5,5,IF(B27=6,3,IF(B27=7,7,255))))))))</f>
-        <v>4</v>
-      </c>
-      <c r="N27" s="7" t="str">
-        <f>IF(AND(B27=L27,C27=M27),"EGAL","")</f>
+      <c r="L27" s="6">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="M27" s="6">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="N27" s="6" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="O27" s="7" t="str">
-        <f>IF(AND(G27=L27,H27=M27),"BON","")</f>
+      <c r="O27" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1" t="str">
-        <f>DEC2BIN(B28, 3)</f>
+        <f t="shared" si="12"/>
         <v>001</v>
       </c>
       <c r="E28" s="1" t="str">
-        <f>DEC2BIN(C28, 3)</f>
-        <v>101</v>
+        <f t="shared" si="13"/>
+        <v>011</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G28">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H28">
         <v>4</v>
       </c>
       <c r="I28" s="1" t="str">
-        <f>DEC2BIN(G28, 3)</f>
-        <v>101</v>
+        <f t="shared" si="14"/>
+        <v>110</v>
       </c>
       <c r="J28" s="1" t="str">
-        <f>DEC2BIN(H28, 3)</f>
+        <f t="shared" si="15"/>
         <v>100</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L28" s="7">
-        <f>IF(C28=0,0,IF(C28=1,4,IF(C28=2,2,IF(C28=3,6,IF(C28=4,1,IF(C28=5,5,IF(C28=6,3,IF(C28=7,7,255))))))))</f>
-        <v>5</v>
-      </c>
-      <c r="M28" s="7">
-        <f>IF(B28=0,0,IF(B28=1,4,IF(B28=2,2,IF(B28=3,6,IF(B28=4,1,IF(B28=5,5,IF(B28=6,3,IF(B28=7,7,255))))))))</f>
-        <v>4</v>
-      </c>
-      <c r="N28" s="7" t="str">
-        <f>IF(AND(B28=L28,C28=M28),"EGAL","")</f>
+      <c r="L28" s="6">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="M28" s="6">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="N28" s="6" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="O28" s="7" t="str">
-        <f>IF(AND(G28=L28,H28=M28),"BON","")</f>
+      <c r="O28" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D29" s="1" t="str">
-        <f>DEC2BIN(B29, 3)</f>
-        <v>010</v>
+        <f t="shared" si="12"/>
+        <v>001</v>
       </c>
       <c r="E29" s="1" t="str">
-        <f>DEC2BIN(C29, 3)</f>
-        <v>001</v>
+        <f t="shared" si="13"/>
+        <v>101</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="G29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I29" s="1" t="str">
-        <f>DEC2BIN(G29, 3)</f>
-        <v>100</v>
+        <f t="shared" si="14"/>
+        <v>101</v>
       </c>
       <c r="J29" s="1" t="str">
-        <f>DEC2BIN(H29, 3)</f>
-        <v>010</v>
-      </c>
-      <c r="K29" t="s">
-        <v>6</v>
-      </c>
-      <c r="L29" s="7">
-        <f>IF(C29=0,0,IF(C29=1,4,IF(C29=2,2,IF(C29=3,6,IF(C29=4,1,IF(C29=5,5,IF(C29=6,3,IF(C29=7,7,255))))))))</f>
-        <v>4</v>
-      </c>
-      <c r="M29" s="7">
-        <f>IF(B29=0,0,IF(B29=1,4,IF(B29=2,2,IF(B29=3,6,IF(B29=4,1,IF(B29=5,5,IF(B29=6,3,IF(B29=7,7,255))))))))</f>
-        <v>2</v>
-      </c>
-      <c r="N29" s="7" t="str">
-        <f>IF(AND(B29=L29,C29=M29),"EGAL","")</f>
+        <f t="shared" si="15"/>
+        <v>100</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L29" s="6">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="M29" s="6">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="N29" s="6" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="O29" s="7" t="str">
-        <f>IF(AND(G29=L29,H29=M29),"BON","")</f>
+      <c r="O29" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D30" s="1" t="str">
-        <f>DEC2BIN(B30, 3)</f>
+        <f t="shared" si="12"/>
         <v>010</v>
       </c>
       <c r="E30" s="1" t="str">
-        <f>DEC2BIN(C30, 3)</f>
-        <v>011</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>001</v>
       </c>
       <c r="G30">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H30">
         <v>2</v>
       </c>
       <c r="I30" s="1" t="str">
-        <f>DEC2BIN(G30, 3)</f>
-        <v>110</v>
+        <f t="shared" si="14"/>
+        <v>100</v>
       </c>
       <c r="J30" s="1" t="str">
-        <f>DEC2BIN(H30, 3)</f>
-        <v>010</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L30" s="7">
-        <f>IF(C30=0,0,IF(C30=1,4,IF(C30=2,2,IF(C30=3,6,IF(C30=4,1,IF(C30=5,5,IF(C30=6,3,IF(C30=7,7,255))))))))</f>
-        <v>6</v>
-      </c>
-      <c r="M30" s="7">
-        <f>IF(B30=0,0,IF(B30=1,4,IF(B30=2,2,IF(B30=3,6,IF(B30=4,1,IF(B30=5,5,IF(B30=6,3,IF(B30=7,7,255))))))))</f>
-        <v>2</v>
-      </c>
-      <c r="N30" s="7" t="str">
-        <f>IF(AND(B30=L30,C30=M30),"EGAL","")</f>
+        <f t="shared" si="15"/>
+        <v>010</v>
+      </c>
+      <c r="K30" t="s">
+        <v>6</v>
+      </c>
+      <c r="L30" s="6">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="M30" s="6">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="N30" s="6" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="O30" s="7" t="str">
-        <f>IF(AND(G30=L30,H30=M30),"BON","")</f>
+      <c r="O30" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D31" s="1" t="str">
-        <f>DEC2BIN(B31, 3)</f>
+        <f t="shared" si="12"/>
         <v>010</v>
       </c>
       <c r="E31" s="1" t="str">
-        <f>DEC2BIN(C31, 3)</f>
-        <v>101</v>
+        <f t="shared" si="13"/>
+        <v>011</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G31">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H31">
         <v>2</v>
       </c>
       <c r="I31" s="1" t="str">
-        <f>DEC2BIN(G31, 3)</f>
-        <v>101</v>
+        <f t="shared" si="14"/>
+        <v>110</v>
       </c>
       <c r="J31" s="1" t="str">
-        <f>DEC2BIN(H31, 3)</f>
+        <f t="shared" si="15"/>
         <v>010</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L31" s="7">
-        <f>IF(C31=0,0,IF(C31=1,4,IF(C31=2,2,IF(C31=3,6,IF(C31=4,1,IF(C31=5,5,IF(C31=6,3,IF(C31=7,7,255))))))))</f>
-        <v>5</v>
-      </c>
-      <c r="M31" s="7">
-        <f>IF(B31=0,0,IF(B31=1,4,IF(B31=2,2,IF(B31=3,6,IF(B31=4,1,IF(B31=5,5,IF(B31=6,3,IF(B31=7,7,255))))))))</f>
-        <v>2</v>
-      </c>
-      <c r="N31" s="7" t="str">
-        <f>IF(AND(B31=L31,C31=M31),"EGAL","")</f>
+      <c r="L31" s="6">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="M31" s="6">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="N31" s="6" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="O31" s="7" t="str">
-        <f>IF(AND(G31=L31,H31=M31),"BON","")</f>
+      <c r="O31" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D32" s="1" t="str">
-        <f>DEC2BIN(B32, 3)</f>
+        <f t="shared" si="12"/>
         <v>010</v>
       </c>
       <c r="E32" s="1" t="str">
-        <f>DEC2BIN(C32, 3)</f>
-        <v>110</v>
+        <f t="shared" si="13"/>
+        <v>101</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G32">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H32">
         <v>2</v>
       </c>
       <c r="I32" s="1" t="str">
-        <f>DEC2BIN(G32, 3)</f>
-        <v>011</v>
+        <f t="shared" si="14"/>
+        <v>101</v>
       </c>
       <c r="J32" s="1" t="str">
-        <f>DEC2BIN(H32, 3)</f>
+        <f t="shared" si="15"/>
         <v>010</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L32" s="7">
-        <f>IF(C32=0,0,IF(C32=1,4,IF(C32=2,2,IF(C32=3,6,IF(C32=4,1,IF(C32=5,5,IF(C32=6,3,IF(C32=7,7,255))))))))</f>
-        <v>3</v>
-      </c>
-      <c r="M32" s="7">
-        <f>IF(B32=0,0,IF(B32=1,4,IF(B32=2,2,IF(B32=3,6,IF(B32=4,1,IF(B32=5,5,IF(B32=6,3,IF(B32=7,7,255))))))))</f>
-        <v>2</v>
-      </c>
-      <c r="N32" s="7" t="str">
-        <f>IF(AND(B32=L32,C32=M32),"EGAL","")</f>
+      <c r="L32" s="6">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="M32" s="6">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="N32" s="6" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="O32" s="7" t="str">
-        <f>IF(AND(G32=L32,H32=M32),"BON","")</f>
+      <c r="O32" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
       <c r="C33">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D33" s="1" t="str">
-        <f>DEC2BIN(B33, 3)</f>
+        <f t="shared" si="12"/>
         <v>010</v>
       </c>
       <c r="E33" s="1" t="str">
-        <f>DEC2BIN(C33, 3)</f>
-        <v>111</v>
+        <f t="shared" si="13"/>
+        <v>110</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G33">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H33">
         <v>2</v>
       </c>
       <c r="I33" s="1" t="str">
-        <f>DEC2BIN(G33, 3)</f>
-        <v>111</v>
+        <f t="shared" si="14"/>
+        <v>011</v>
       </c>
       <c r="J33" s="1" t="str">
-        <f>DEC2BIN(H33, 3)</f>
+        <f t="shared" si="15"/>
         <v>010</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L33" s="7">
-        <f>IF(C33=0,0,IF(C33=1,4,IF(C33=2,2,IF(C33=3,6,IF(C33=4,1,IF(C33=5,5,IF(C33=6,3,IF(C33=7,7,255))))))))</f>
-        <v>7</v>
-      </c>
-      <c r="M33" s="7">
-        <f>IF(B33=0,0,IF(B33=1,4,IF(B33=2,2,IF(B33=3,6,IF(B33=4,1,IF(B33=5,5,IF(B33=6,3,IF(B33=7,7,255))))))))</f>
-        <v>2</v>
-      </c>
-      <c r="N33" s="7" t="str">
-        <f>IF(AND(B33=L33,C33=M33),"EGAL","")</f>
+      <c r="L33" s="6">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="M33" s="6">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="N33" s="6" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="O33" s="7" t="str">
-        <f>IF(AND(G33=L33,H33=M33),"BON","")</f>
+      <c r="O33" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D34" s="1" t="str">
-        <f>DEC2BIN(B34, 3)</f>
-        <v>011</v>
+        <f t="shared" si="12"/>
+        <v>010</v>
       </c>
       <c r="E34" s="1" t="str">
-        <f>DEC2BIN(C34, 3)</f>
-        <v>001</v>
+        <f t="shared" si="13"/>
+        <v>111</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H34">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I34" s="1" t="str">
-        <f>DEC2BIN(G34, 3)</f>
-        <v>100</v>
+        <f t="shared" si="14"/>
+        <v>111</v>
       </c>
       <c r="J34" s="1" t="str">
-        <f>DEC2BIN(H34, 3)</f>
-        <v>110</v>
-      </c>
-      <c r="K34" t="s">
-        <v>6</v>
-      </c>
-      <c r="L34" s="7">
-        <f>IF(C34=0,0,IF(C34=1,4,IF(C34=2,2,IF(C34=3,6,IF(C34=4,1,IF(C34=5,5,IF(C34=6,3,IF(C34=7,7,255))))))))</f>
-        <v>4</v>
-      </c>
-      <c r="M34" s="7">
-        <f>IF(B34=0,0,IF(B34=1,4,IF(B34=2,2,IF(B34=3,6,IF(B34=4,1,IF(B34=5,5,IF(B34=6,3,IF(B34=7,7,255))))))))</f>
-        <v>6</v>
-      </c>
-      <c r="N34" s="7" t="str">
-        <f>IF(AND(B34=L34,C34=M34),"EGAL","")</f>
+        <f t="shared" si="15"/>
+        <v>010</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L34" s="6">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+      <c r="M34" s="6">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="N34" s="6" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="O34" s="7" t="str">
-        <f>IF(AND(G34=L34,H34=M34),"BON","")</f>
+      <c r="O34" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1" t="str">
-        <f>DEC2BIN(B35, 3)</f>
+        <f t="shared" si="12"/>
         <v>011</v>
       </c>
       <c r="E35" s="1" t="str">
-        <f>DEC2BIN(C35, 3)</f>
-        <v>011</v>
+        <f t="shared" si="13"/>
+        <v>001</v>
       </c>
       <c r="G35">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H35">
         <v>6</v>
       </c>
       <c r="I35" s="1" t="str">
-        <f>DEC2BIN(G35, 3)</f>
-        <v>110</v>
+        <f t="shared" si="14"/>
+        <v>100</v>
       </c>
       <c r="J35" s="1" t="str">
-        <f>DEC2BIN(H35, 3)</f>
-        <v>110</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L35" s="7">
-        <f>IF(C35=0,0,IF(C35=1,4,IF(C35=2,2,IF(C35=3,6,IF(C35=4,1,IF(C35=5,5,IF(C35=6,3,IF(C35=7,7,255))))))))</f>
-        <v>6</v>
-      </c>
-      <c r="M35" s="7">
-        <f>IF(B35=0,0,IF(B35=1,4,IF(B35=2,2,IF(B35=3,6,IF(B35=4,1,IF(B35=5,5,IF(B35=6,3,IF(B35=7,7,255))))))))</f>
-        <v>6</v>
-      </c>
-      <c r="N35" s="7" t="str">
-        <f>IF(AND(B35=L35,C35=M35),"EGAL","")</f>
+        <f t="shared" si="15"/>
+        <v>110</v>
+      </c>
+      <c r="K35" t="s">
+        <v>6</v>
+      </c>
+      <c r="L35" s="6">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="M35" s="6">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="N35" s="6" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="O35" s="7" t="str">
-        <f>IF(AND(G35=L35,H35=M35),"BON","")</f>
+      <c r="O35" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B36">
         <v>3</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D36" s="1" t="str">
-        <f>DEC2BIN(B36, 3)</f>
+        <f t="shared" si="12"/>
         <v>011</v>
       </c>
       <c r="E36" s="1" t="str">
-        <f>DEC2BIN(C36, 3)</f>
-        <v>101</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>011</v>
       </c>
       <c r="G36">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H36">
         <v>6</v>
       </c>
       <c r="I36" s="1" t="str">
-        <f>DEC2BIN(G36, 3)</f>
-        <v>101</v>
+        <f t="shared" si="14"/>
+        <v>110</v>
       </c>
       <c r="J36" s="1" t="str">
-        <f>DEC2BIN(H36, 3)</f>
+        <f t="shared" si="15"/>
         <v>110</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L36" s="7">
-        <f>IF(C36=0,0,IF(C36=1,4,IF(C36=2,2,IF(C36=3,6,IF(C36=4,1,IF(C36=5,5,IF(C36=6,3,IF(C36=7,7,255))))))))</f>
-        <v>5</v>
-      </c>
-      <c r="M36" s="7">
-        <f>IF(B36=0,0,IF(B36=1,4,IF(B36=2,2,IF(B36=3,6,IF(B36=4,1,IF(B36=5,5,IF(B36=6,3,IF(B36=7,7,255))))))))</f>
-        <v>6</v>
-      </c>
-      <c r="N36" s="7" t="str">
-        <f>IF(AND(B36=L36,C36=M36),"EGAL","")</f>
+        <v>6</v>
+      </c>
+      <c r="L36" s="6">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="M36" s="6">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="N36" s="6" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="O36" s="7" t="str">
-        <f>IF(AND(G36=L36,H36=M36),"BON","")</f>
+      <c r="O36" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D37" s="1" t="str">
-        <f>DEC2BIN(B37, 3)</f>
-        <v>100</v>
+        <f t="shared" si="12"/>
+        <v>011</v>
       </c>
       <c r="E37" s="1" t="str">
-        <f>DEC2BIN(C37, 3)</f>
-        <v>001</v>
-      </c>
-      <c r="F37" t="s">
-        <v>6</v>
+        <f t="shared" si="13"/>
+        <v>101</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="G37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f>DEC2BIN(G37, 3)</f>
-        <v>100</v>
+        <f t="shared" si="14"/>
+        <v>101</v>
       </c>
       <c r="J37" s="1" t="str">
-        <f>DEC2BIN(H37, 3)</f>
-        <v>001</v>
-      </c>
-      <c r="L37" s="7">
-        <f>IF(C37=0,0,IF(C37=1,4,IF(C37=2,2,IF(C37=3,6,IF(C37=4,1,IF(C37=5,5,IF(C37=6,3,IF(C37=7,7,255))))))))</f>
-        <v>4</v>
-      </c>
-      <c r="M37" s="7">
-        <f>IF(B37=0,0,IF(B37=1,4,IF(B37=2,2,IF(B37=3,6,IF(B37=4,1,IF(B37=5,5,IF(B37=6,3,IF(B37=7,7,255))))))))</f>
-        <v>1</v>
-      </c>
-      <c r="N37" s="7" t="str">
-        <f>IF(AND(B37=L37,C37=M37),"EGAL","")</f>
-        <v>EGAL</v>
-      </c>
-      <c r="O37" s="7" t="str">
-        <f>IF(AND(G37=L37,H37=M37),"BON","")</f>
+        <f t="shared" si="15"/>
+        <v>110</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L37" s="6">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="M37" s="6">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="N37" s="6" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="O37" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B38">
         <v>4</v>
       </c>
       <c r="C38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D38" s="1" t="str">
-        <f>DEC2BIN(B38, 3)</f>
+        <f t="shared" si="12"/>
         <v>100</v>
       </c>
       <c r="E38" s="1" t="str">
-        <f>DEC2BIN(C38, 3)</f>
-        <v>011</v>
+        <f t="shared" si="13"/>
+        <v>001</v>
       </c>
       <c r="F38" t="s">
         <v>6</v>
       </c>
       <c r="G38">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H38">
         <v>1</v>
       </c>
       <c r="I38" s="1" t="str">
-        <f>DEC2BIN(G38, 3)</f>
-        <v>110</v>
+        <f t="shared" si="14"/>
+        <v>100</v>
       </c>
       <c r="J38" s="1" t="str">
-        <f>DEC2BIN(H38, 3)</f>
+        <f t="shared" si="15"/>
         <v>001</v>
       </c>
-      <c r="K38" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L38" s="7">
-        <f>IF(C38=0,0,IF(C38=1,4,IF(C38=2,2,IF(C38=3,6,IF(C38=4,1,IF(C38=5,5,IF(C38=6,3,IF(C38=7,7,255))))))))</f>
-        <v>6</v>
-      </c>
-      <c r="M38" s="7">
-        <f>IF(B38=0,0,IF(B38=1,4,IF(B38=2,2,IF(B38=3,6,IF(B38=4,1,IF(B38=5,5,IF(B38=6,3,IF(B38=7,7,255))))))))</f>
-        <v>1</v>
-      </c>
-      <c r="N38" s="7" t="str">
-        <f>IF(AND(B38=L38,C38=M38),"EGAL","")</f>
-        <v/>
-      </c>
-      <c r="O38" s="7" t="str">
-        <f>IF(AND(G38=L38,H38=M38),"BON","")</f>
+      <c r="L38" s="6">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="M38" s="6">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="N38" s="6" t="str">
+        <f t="shared" si="18"/>
+        <v>EGAL</v>
+      </c>
+      <c r="O38" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B39">
         <v>4</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D39" s="1" t="str">
-        <f>DEC2BIN(B39, 3)</f>
+        <f t="shared" si="12"/>
         <v>100</v>
       </c>
       <c r="E39" s="1" t="str">
-        <f>DEC2BIN(C39, 3)</f>
-        <v>101</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>011</v>
+      </c>
+      <c r="F39" t="s">
+        <v>6</v>
       </c>
       <c r="G39">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H39">
         <v>1</v>
       </c>
       <c r="I39" s="1" t="str">
-        <f>DEC2BIN(G39, 3)</f>
-        <v>101</v>
+        <f t="shared" si="14"/>
+        <v>110</v>
       </c>
       <c r="J39" s="1" t="str">
-        <f>DEC2BIN(H39, 3)</f>
+        <f t="shared" si="15"/>
         <v>001</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L39" s="7">
-        <f>IF(C39=0,0,IF(C39=1,4,IF(C39=2,2,IF(C39=3,6,IF(C39=4,1,IF(C39=5,5,IF(C39=6,3,IF(C39=7,7,255))))))))</f>
-        <v>5</v>
-      </c>
-      <c r="M39" s="7">
-        <f>IF(B39=0,0,IF(B39=1,4,IF(B39=2,2,IF(B39=3,6,IF(B39=4,1,IF(B39=5,5,IF(B39=6,3,IF(B39=7,7,255))))))))</f>
-        <v>1</v>
-      </c>
-      <c r="N39" s="7" t="str">
-        <f>IF(AND(B39=L39,C39=M39),"EGAL","")</f>
+        <v>6</v>
+      </c>
+      <c r="L39" s="6">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="M39" s="6">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="N39" s="6" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="O39" s="7" t="str">
-        <f>IF(AND(G39=L39,H39=M39),"BON","")</f>
+      <c r="O39" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B40">
         <v>4</v>
       </c>
       <c r="C40">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D40" s="1" t="str">
-        <f>DEC2BIN(B40, 3)</f>
+        <f t="shared" si="12"/>
         <v>100</v>
       </c>
       <c r="E40" s="1" t="str">
-        <f>DEC2BIN(C40, 3)</f>
-        <v>111</v>
-      </c>
-      <c r="F40" t="s">
-        <v>6</v>
+        <f t="shared" si="13"/>
+        <v>101</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="G40">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H40">
         <v>1</v>
       </c>
       <c r="I40" s="1" t="str">
-        <f>DEC2BIN(G40, 3)</f>
-        <v>111</v>
+        <f t="shared" si="14"/>
+        <v>101</v>
       </c>
       <c r="J40" s="1" t="str">
-        <f>DEC2BIN(H40, 3)</f>
+        <f t="shared" si="15"/>
         <v>001</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L40" s="7">
-        <f>IF(C40=0,0,IF(C40=1,4,IF(C40=2,2,IF(C40=3,6,IF(C40=4,1,IF(C40=5,5,IF(C40=6,3,IF(C40=7,7,255))))))))</f>
-        <v>7</v>
-      </c>
-      <c r="M40" s="7">
-        <f>IF(B40=0,0,IF(B40=1,4,IF(B40=2,2,IF(B40=3,6,IF(B40=4,1,IF(B40=5,5,IF(B40=6,3,IF(B40=7,7,255))))))))</f>
-        <v>1</v>
-      </c>
-      <c r="N40" s="7" t="str">
-        <f>IF(AND(B40=L40,C40=M40),"EGAL","")</f>
+        <v>0</v>
+      </c>
+      <c r="L40" s="6">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="M40" s="6">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="N40" s="6" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="O40" s="7" t="str">
-        <f>IF(AND(G40=L40,H40=M40),"BON","")</f>
+      <c r="O40" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D41" s="1" t="str">
-        <f>DEC2BIN(B41, 3)</f>
-        <v>101</v>
+        <f t="shared" si="12"/>
+        <v>100</v>
       </c>
       <c r="E41" s="1" t="str">
-        <f>DEC2BIN(C41, 3)</f>
-        <v>011</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>111</v>
+      </c>
+      <c r="F41" t="s">
+        <v>6</v>
       </c>
       <c r="G41">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H41">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I41" s="1" t="str">
-        <f>DEC2BIN(G41, 3)</f>
-        <v>110</v>
+        <f t="shared" si="14"/>
+        <v>111</v>
       </c>
       <c r="J41" s="1" t="str">
-        <f>DEC2BIN(H41, 3)</f>
-        <v>101</v>
+        <f t="shared" si="15"/>
+        <v>001</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L41" s="7">
-        <f>IF(C41=0,0,IF(C41=1,4,IF(C41=2,2,IF(C41=3,6,IF(C41=4,1,IF(C41=5,5,IF(C41=6,3,IF(C41=7,7,255))))))))</f>
-        <v>6</v>
-      </c>
-      <c r="M41" s="7">
-        <f>IF(B41=0,0,IF(B41=1,4,IF(B41=2,2,IF(B41=3,6,IF(B41=4,1,IF(B41=5,5,IF(B41=6,3,IF(B41=7,7,255))))))))</f>
-        <v>5</v>
-      </c>
-      <c r="N41" s="7" t="str">
-        <f>IF(AND(B41=L41,C41=M41),"EGAL","")</f>
+        <v>6</v>
+      </c>
+      <c r="L41" s="6">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+      <c r="M41" s="6">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="N41" s="6" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="O41" s="7" t="str">
-        <f>IF(AND(G41=L41,H41=M41),"BON","")</f>
+      <c r="O41" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B42">
         <v>5</v>
       </c>
       <c r="C42">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D42" s="1" t="str">
-        <f>DEC2BIN(B42, 3)</f>
+        <f t="shared" si="12"/>
         <v>101</v>
       </c>
       <c r="E42" s="1" t="str">
-        <f>DEC2BIN(C42, 3)</f>
-        <v>111</v>
+        <f t="shared" si="13"/>
+        <v>011</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G42">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H42">
         <v>5</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f>DEC2BIN(G42, 3)</f>
-        <v>111</v>
+        <f t="shared" si="14"/>
+        <v>110</v>
       </c>
       <c r="J42" s="1" t="str">
-        <f>DEC2BIN(H42, 3)</f>
+        <f t="shared" si="15"/>
         <v>101</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L42" s="7">
-        <f t="shared" ref="L42" si="8">IF(C42=0,0,IF(C42=1,4,IF(C42=2,2,IF(C42=3,6,IF(C42=4,1,IF(C42=5,5,IF(C42=6,3,IF(C42=7,7,255))))))))</f>
-        <v>7</v>
-      </c>
-      <c r="M42" s="7">
-        <f t="shared" ref="M42" si="9">IF(B42=0,0,IF(B42=1,4,IF(B42=2,2,IF(B42=3,6,IF(B42=4,1,IF(B42=5,5,IF(B42=6,3,IF(B42=7,7,255))))))))</f>
-        <v>5</v>
-      </c>
-      <c r="N42" s="7" t="str">
-        <f t="shared" ref="N42" si="10">IF(AND(B42=L42,C42=M42),"EGAL","")</f>
+      <c r="L42" s="6">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="M42" s="6">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="N42" s="6" t="str">
+        <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="O42" s="7" t="str">
-        <f>IF(AND(G42=L42,H42=M42),"BON","")</f>
+      <c r="O42" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B43">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C43">
         <v>7</v>
       </c>
       <c r="D43" s="1" t="str">
-        <f>DEC2BIN(B43, 3)</f>
-        <v>110</v>
+        <f t="shared" si="12"/>
+        <v>101</v>
       </c>
       <c r="E43" s="1" t="str">
-        <f>DEC2BIN(C43, 3)</f>
+        <f t="shared" si="13"/>
         <v>111</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G43">
         <v>7</v>
       </c>
       <c r="H43">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I43" s="1" t="str">
-        <f>DEC2BIN(G43, 3)</f>
+        <f t="shared" si="14"/>
         <v>111</v>
       </c>
       <c r="J43" s="1" t="str">
-        <f>DEC2BIN(H43, 3)</f>
-        <v>011</v>
+        <f t="shared" si="15"/>
+        <v>101</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L43" s="7">
-        <f t="shared" ref="L43" si="11">IF(C43=0,0,IF(C43=1,4,IF(C43=2,2,IF(C43=3,6,IF(C43=4,1,IF(C43=5,5,IF(C43=6,3,IF(C43=7,7,255))))))))</f>
-        <v>7</v>
-      </c>
-      <c r="M43" s="7">
-        <f t="shared" ref="M43" si="12">IF(B43=0,0,IF(B43=1,4,IF(B43=2,2,IF(B43=3,6,IF(B43=4,1,IF(B43=5,5,IF(B43=6,3,IF(B43=7,7,255))))))))</f>
-        <v>3</v>
-      </c>
-      <c r="N43" s="7" t="str">
-        <f t="shared" ref="N43" si="13">IF(AND(B43=L43,C43=M43),"EGAL","")</f>
+        <v>0</v>
+      </c>
+      <c r="L43" s="6">
+        <f t="shared" ref="L43" si="20">IF(C43=0,0,IF(C43=1,4,IF(C43=2,2,IF(C43=3,6,IF(C43=4,1,IF(C43=5,5,IF(C43=6,3,IF(C43=7,7,255))))))))</f>
+        <v>7</v>
+      </c>
+      <c r="M43" s="6">
+        <f t="shared" ref="M43" si="21">IF(B43=0,0,IF(B43=1,4,IF(B43=2,2,IF(B43=3,6,IF(B43=4,1,IF(B43=5,5,IF(B43=6,3,IF(B43=7,7,255))))))))</f>
+        <v>5</v>
+      </c>
+      <c r="N43" s="6" t="str">
+        <f t="shared" ref="N43" si="22">IF(AND(B43=L43,C43=M43),"EGAL","")</f>
         <v/>
       </c>
-      <c r="O43" s="7" t="str">
-        <f t="shared" ref="O43" si="14">IF(AND(G43=L43,H43=M43),"BON","")</f>
+      <c r="O43" s="6" t="str">
+        <f t="shared" si="19"/>
         <v>BON</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C44">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D44" s="1" t="str">
-        <f>DEC2BIN(B44, 3)</f>
-        <v>101</v>
+        <f t="shared" si="12"/>
+        <v>110</v>
       </c>
       <c r="E44" s="1" t="str">
-        <f>DEC2BIN(C44, 3)</f>
-        <v>101</v>
+        <f t="shared" si="13"/>
+        <v>111</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G44">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H44">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I44" s="1" t="str">
-        <f>DEC2BIN(G44, 3)</f>
-        <v>101</v>
+        <f t="shared" si="14"/>
+        <v>111</v>
       </c>
       <c r="J44" s="1" t="str">
-        <f>DEC2BIN(H44, 3)</f>
-        <v>101</v>
-      </c>
-      <c r="L44" s="7">
-        <f>IF(C44=0,0,IF(C44=1,4,IF(C44=2,2,IF(C44=3,6,IF(C44=4,1,IF(C44=5,5,IF(C44=6,3,IF(C44=7,7,255))))))))</f>
-        <v>5</v>
-      </c>
-      <c r="M44" s="7">
-        <f>IF(B44=0,0,IF(B44=1,4,IF(B44=2,2,IF(B44=3,6,IF(B44=4,1,IF(B44=5,5,IF(B44=6,3,IF(B44=7,7,255))))))))</f>
-        <v>5</v>
-      </c>
-      <c r="N44" s="7" t="str">
-        <f>IF(AND(B44=L44,C44=M44),"EGAL","")</f>
-        <v>EGAL</v>
-      </c>
-      <c r="O44" s="7" t="str">
-        <f>IF(AND(G44=L44,H44=M44),"BON","")</f>
+        <f t="shared" si="15"/>
+        <v>011</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L44" s="6">
+        <f t="shared" ref="L44" si="23">IF(C44=0,0,IF(C44=1,4,IF(C44=2,2,IF(C44=3,6,IF(C44=4,1,IF(C44=5,5,IF(C44=6,3,IF(C44=7,7,255))))))))</f>
+        <v>7</v>
+      </c>
+      <c r="M44" s="6">
+        <f t="shared" ref="M44" si="24">IF(B44=0,0,IF(B44=1,4,IF(B44=2,2,IF(B44=3,6,IF(B44=4,1,IF(B44=5,5,IF(B44=6,3,IF(B44=7,7,255))))))))</f>
+        <v>3</v>
+      </c>
+      <c r="N44" s="6" t="str">
+        <f t="shared" ref="N44" si="25">IF(AND(B44=L44,C44=M44),"EGAL","")</f>
+        <v/>
+      </c>
+      <c r="O44" s="6" t="str">
+        <f t="shared" ref="O44" si="26">IF(AND(G44=L44,H44=M44),"BON","")</f>
         <v>BON</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
+        <v>32</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>101</v>
+      </c>
+      <c r="E45" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>101</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>5</v>
+      </c>
+      <c r="H45">
+        <v>5</v>
+      </c>
+      <c r="I45" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v>101</v>
+      </c>
+      <c r="J45" s="1" t="str">
+        <f t="shared" si="15"/>
+        <v>101</v>
+      </c>
+      <c r="L45" s="6">
+        <f>IF(C45=0,0,IF(C45=1,4,IF(C45=2,2,IF(C45=3,6,IF(C45=4,1,IF(C45=5,5,IF(C45=6,3,IF(C45=7,7,255))))))))</f>
+        <v>5</v>
+      </c>
+      <c r="M45" s="6">
+        <f>IF(B45=0,0,IF(B45=1,4,IF(B45=2,2,IF(B45=3,6,IF(B45=4,1,IF(B45=5,5,IF(B45=6,3,IF(B45=7,7,255))))))))</f>
+        <v>5</v>
+      </c>
+      <c r="N45" s="6" t="str">
+        <f>IF(AND(B45=L45,C45=M45),"EGAL","")</f>
+        <v>EGAL</v>
+      </c>
+      <c r="O45" s="6" t="str">
+        <f>IF(AND(G45=L45,H45=M45),"BON","")</f>
+        <v>BON</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>34</v>
       </c>
-      <c r="B45">
-        <v>6</v>
-      </c>
-      <c r="C45">
-        <v>3</v>
-      </c>
-      <c r="D45" s="1" t="str">
-        <f>DEC2BIN(B45, 3)</f>
-        <v>110</v>
-      </c>
-      <c r="E45" s="1" t="str">
-        <f>DEC2BIN(C45, 3)</f>
+      <c r="B46">
+        <v>6</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>110</v>
+      </c>
+      <c r="E46" s="1" t="str">
+        <f t="shared" si="13"/>
         <v>011</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>6</v>
-      </c>
-      <c r="H45">
-        <v>3</v>
-      </c>
-      <c r="I45" s="1" t="str">
-        <f>DEC2BIN(G45, 3)</f>
-        <v>110</v>
-      </c>
-      <c r="J45" s="1" t="str">
-        <f>DEC2BIN(H45, 3)</f>
+      <c r="F46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>6</v>
+      </c>
+      <c r="H46">
+        <v>3</v>
+      </c>
+      <c r="I46" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v>110</v>
+      </c>
+      <c r="J46" s="1" t="str">
+        <f t="shared" si="15"/>
         <v>011</v>
       </c>
-      <c r="L45" s="7">
-        <f t="shared" ref="L45" si="15">IF(C45=0,0,IF(C45=1,4,IF(C45=2,2,IF(C45=3,6,IF(C45=4,1,IF(C45=5,5,IF(C45=6,3,IF(C45=7,7,255))))))))</f>
-        <v>6</v>
-      </c>
-      <c r="M45" s="7">
-        <f t="shared" ref="M45" si="16">IF(B45=0,0,IF(B45=1,4,IF(B45=2,2,IF(B45=3,6,IF(B45=4,1,IF(B45=5,5,IF(B45=6,3,IF(B45=7,7,255))))))))</f>
-        <v>3</v>
-      </c>
-      <c r="N45" s="7" t="str">
-        <f t="shared" ref="N45" si="17">IF(AND(B45=L45,C45=M45),"EGAL","")</f>
+      <c r="L46" s="6">
+        <f t="shared" ref="L46" si="27">IF(C46=0,0,IF(C46=1,4,IF(C46=2,2,IF(C46=3,6,IF(C46=4,1,IF(C46=5,5,IF(C46=6,3,IF(C46=7,7,255))))))))</f>
+        <v>6</v>
+      </c>
+      <c r="M46" s="6">
+        <f t="shared" ref="M46" si="28">IF(B46=0,0,IF(B46=1,4,IF(B46=2,2,IF(B46=3,6,IF(B46=4,1,IF(B46=5,5,IF(B46=6,3,IF(B46=7,7,255))))))))</f>
+        <v>3</v>
+      </c>
+      <c r="N46" s="6" t="str">
+        <f t="shared" ref="N46" si="29">IF(AND(B46=L46,C46=M46),"EGAL","")</f>
         <v>EGAL</v>
       </c>
-      <c r="O45" s="7" t="str">
-        <f t="shared" ref="O45" si="18">IF(AND(G45=L45,H45=M45),"BON","")</f>
+      <c r="O46" s="6" t="str">
+        <f t="shared" ref="O46" si="30">IF(AND(G46=L46,H46=M46),"BON","")</f>
         <v>BON</v>
       </c>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E50" s="1"/>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Réalignement fonctionnel version machine d'état même si de petits artéfacts persistent notament dans la jonction retrieve/realign surtout si realign arrive sur la ligne trop vite...
</commit_message>
<xml_diff>
--- a/_01-docs/_01-userDoc/documentionProjetToWeb/source/advanced/simplificationCapteur191214_1518.xlsx
+++ b/_01-docs/_01-userDoc/documentionProjetToWeb/source/advanced/simplificationCapteur191214_1518.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MountWD\Donnees\ODJ\008_iao_wrk\VoRoboticsAsso\00-AutresProjetsDuLab\0025-permiC_2019\project\_01-docs\_01-userDoc\documentionProjetToWeb\source\advanced\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C2062C-6EEF-43AD-BA61-6D6D888D7B05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A8332D-DB5E-4BB3-BF73-67DF6FBD0561}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="1" xr2:uid="{85A47218-88F4-4F6A-A7B0-57E7AE9DD31F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="33">
   <si>
     <t>NON</t>
   </si>
@@ -121,9 +121,6 @@
     <t>incidence max 77°</t>
   </si>
   <si>
-    <t>S2 mais en déplaçant le ou 1,1 à la fin après les autres test</t>
-  </si>
-  <si>
     <t>incidence max 85°</t>
   </si>
   <si>
@@ -133,7 +130,7 @@
     <t>incidence max 74°</t>
   </si>
   <si>
-    <t>S</t>
+    <t>S2 avec choix droite gauche aléatoire dans un premier temps</t>
   </si>
 </sst>
 </file>
@@ -149,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +165,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -181,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -197,7 +206,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -533,10 +548,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="7"/>
+      <c r="F1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="10"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" t="s">
@@ -2390,10 +2405,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E56ABBBC-22BD-47C7-9A9F-76F52387221E}">
-  <dimension ref="A1:T51"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2420,7 +2435,7 @@
     <col min="22" max="22" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2430,12 +2445,12 @@
       <c r="H1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
+      <c r="L1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
       <c r="Q1" t="s">
         <v>11</v>
       </c>
@@ -2443,7 +2458,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2481,7 +2496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2532,11 +2547,11 @@
       <c r="Q3">
         <v>2</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2587,11 +2602,11 @@
       <c r="Q4">
         <v>3</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2642,14 +2657,14 @@
       <c r="Q5">
         <v>4</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="S5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2710,7 +2725,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -2761,14 +2776,14 @@
       <c r="Q7">
         <v>6</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="7" t="s">
         <v>18</v>
       </c>
       <c r="S7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2819,14 +2834,14 @@
       <c r="Q8">
         <v>7</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" s="7" t="s">
         <v>18</v>
       </c>
       <c r="S8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12</v>
       </c>
@@ -2884,7 +2899,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>14</v>
       </c>
@@ -2935,17 +2950,14 @@
       <c r="Q10">
         <v>9</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10" s="7" t="s">
         <v>18</v>
       </c>
       <c r="S10" t="s">
         <v>28</v>
       </c>
-      <c r="T10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15</v>
       </c>
@@ -2996,14 +3008,14 @@
       <c r="Q11">
         <v>10</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11" s="7" t="s">
         <v>18</v>
       </c>
       <c r="S11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>17</v>
       </c>
@@ -3055,10 +3067,10 @@
         <v>11</v>
       </c>
       <c r="R12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>25</v>
       </c>
@@ -3109,14 +3121,14 @@
       <c r="Q13">
         <v>12</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13" s="7" t="s">
         <v>18</v>
       </c>
       <c r="S13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>26</v>
       </c>
@@ -3167,11 +3179,11 @@
       <c r="Q14">
         <v>13</v>
       </c>
-      <c r="R14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R14" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>36</v>
       </c>
@@ -3222,18 +3234,34 @@
       <c r="Q15">
         <v>14</v>
       </c>
-      <c r="R15" t="s">
+      <c r="R15" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="S15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -4457,8 +4485,9 @@
       <c r="E51" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="L1:O1"/>
+    <mergeCell ref="A16:R16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>